<commit_message>
include usage example in API intro
</commit_message>
<xml_diff>
--- a/msl/examples/equipment/example.xlsx
+++ b/msl/examples/equipment/example.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.borbely\code\git\msl-equipment\msl\examples\equipment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\msl-equipment\msl\examples\equipment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
     <sheet name="Connections" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,9 +69,6 @@
     <t>Model No.</t>
   </si>
   <si>
-    <t>AAAAAA</t>
-  </si>
-  <si>
     <t>Keysight</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>3468A</t>
   </si>
   <si>
-    <t>CCCCCC</t>
-  </si>
-  <si>
     <t>5 ½ digit DMM</t>
   </si>
   <si>
@@ -96,15 +90,9 @@
     <t>5492BGPIB</t>
   </si>
   <si>
-    <t>DDDDDD</t>
-  </si>
-  <si>
     <t>Keithley</t>
   </si>
   <si>
-    <t>EEEEEE</t>
-  </si>
-  <si>
     <t>7 ½ digit DMM</t>
   </si>
   <si>
@@ -120,19 +108,31 @@
     <t>MY54506462</t>
   </si>
   <si>
-    <t>USB::0x7B1A::0x0381::AAAAAA</t>
-  </si>
-  <si>
     <t>baud_rate=9600; data_bits=8</t>
   </si>
   <si>
     <t>3458A</t>
   </si>
   <si>
-    <t>FFFFFF</t>
-  </si>
-  <si>
-    <t>USB::0x9D0A::0x2217::FFFFFF</t>
+    <t>D7D59860</t>
+  </si>
+  <si>
+    <t>8BB438A7</t>
+  </si>
+  <si>
+    <t>51957DB9</t>
+  </si>
+  <si>
+    <t>2CAD4BC6</t>
+  </si>
+  <si>
+    <t>USB::0x7B1A::0x0381::D7D59860</t>
+  </si>
+  <si>
+    <t>MY24339283</t>
+  </si>
+  <si>
+    <t>USB::0x9D0A::0x2217::MY24339283</t>
   </si>
 </sst>
 </file>
@@ -542,15 +542,15 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
@@ -564,7 +564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -572,80 +572,80 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="B6" s="4">
         <v>2002</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -660,20 +660,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="6"/>
-    <col min="9" max="9" width="43.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="15.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.86328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.73046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.1328125" style="6"/>
+    <col min="9" max="9" width="43.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
@@ -693,7 +693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -701,81 +701,81 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4">
         <v>2002</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>9</v>
@@ -785,12 +785,12 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>34</v>
@@ -803,7 +803,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -811,7 +811,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -819,7 +819,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
@@ -830,7 +830,7 @@
       <c r="H10"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="12"/>
       <c r="B11" s="8"/>
       <c r="C11" s="12"/>

</xml_diff>